<commit_message>
Added: PCA and LDA transformed data
</commit_message>
<xml_diff>
--- a/data/mixture/3 solutions/PCA.xlsx
+++ b/data/mixture/3 solutions/PCA.xlsx
@@ -452,10 +452,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-22.58364190325597</v>
+        <v>22.58364190325597</v>
       </c>
       <c r="B2" t="n">
-        <v>56.13496713645613</v>
+        <v>-56.13496713645615</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -463,10 +463,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-43.6053335980903</v>
+        <v>43.60533359809029</v>
       </c>
       <c r="B3" t="n">
-        <v>24.37124529499844</v>
+        <v>-24.37124529499845</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -474,10 +474,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-31.77247806104575</v>
+        <v>31.77247806104575</v>
       </c>
       <c r="B4" t="n">
-        <v>-43.89449190627566</v>
+        <v>43.89449190627568</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -485,10 +485,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-36.22098572794811</v>
+        <v>36.22098572794811</v>
       </c>
       <c r="B5" t="n">
-        <v>-61.79061866308646</v>
+        <v>61.79061866308648</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -496,10 +496,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-38.43087430308902</v>
+        <v>38.43087430308902</v>
       </c>
       <c r="B6" t="n">
-        <v>-65.39004204615277</v>
+        <v>65.39004204615279</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -507,10 +507,10 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-40.38613145275495</v>
+        <v>40.38613145275494</v>
       </c>
       <c r="B7" t="n">
-        <v>-69.56176818315581</v>
+        <v>69.56176818315582</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -518,10 +518,10 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-42.0057982628362</v>
+        <v>42.00579826283618</v>
       </c>
       <c r="B8" t="n">
-        <v>-76.68794164859355</v>
+        <v>76.68794164859358</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
@@ -529,10 +529,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-52.19136477635873</v>
+        <v>52.19136477635872</v>
       </c>
       <c r="B9" t="n">
-        <v>-99.25097515595088</v>
+        <v>99.25097515595091</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -540,10 +540,10 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-68.88199345259926</v>
+        <v>68.88199345259925</v>
       </c>
       <c r="B10" t="n">
-        <v>-118.948943988071</v>
+        <v>118.948943988071</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
@@ -551,10 +551,10 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-96.86753007657387</v>
+        <v>96.86753007657389</v>
       </c>
       <c r="B11" t="n">
-        <v>-135.4551514497722</v>
+        <v>135.4551514497722</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
@@ -562,10 +562,10 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-34.12364113983869</v>
+        <v>34.12364113983868</v>
       </c>
       <c r="B12" t="n">
-        <v>-30.74516523407399</v>
+        <v>30.745165234074</v>
       </c>
       <c r="C12" t="n">
         <v>1</v>
@@ -573,10 +573,10 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-44.04136021147246</v>
+        <v>44.04136021147245</v>
       </c>
       <c r="B13" t="n">
-        <v>24.48508649461824</v>
+        <v>-24.48508649461825</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
@@ -584,10 +584,10 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-22.56625043833582</v>
+        <v>22.56625043833582</v>
       </c>
       <c r="B14" t="n">
-        <v>55.61746398950656</v>
+        <v>-55.61746398950658</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
@@ -595,10 +595,10 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-33.87625747777388</v>
+        <v>33.87625747777388</v>
       </c>
       <c r="B15" t="n">
-        <v>-30.70664538771632</v>
+        <v>30.70664538771633</v>
       </c>
       <c r="C15" t="n">
         <v>1</v>
@@ -606,10 +606,10 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-43.18716545869167</v>
+        <v>43.18716545869167</v>
       </c>
       <c r="B16" t="n">
-        <v>24.15976399227023</v>
+        <v>-24.15976399227024</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
@@ -617,10 +617,10 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-22.74602341084481</v>
+        <v>22.74602341084481</v>
       </c>
       <c r="B17" t="n">
-        <v>57.30453828288846</v>
+        <v>-57.30453828288847</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
@@ -628,10 +628,10 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-34.303773282847</v>
+        <v>34.30377328284699</v>
       </c>
       <c r="B18" t="n">
-        <v>-30.7732134180763</v>
+        <v>30.77321341807631</v>
       </c>
       <c r="C18" t="n">
         <v>1</v>
@@ -639,10 +639,10 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-43.44151134737071</v>
+        <v>43.44151134737073</v>
       </c>
       <c r="B19" t="n">
-        <v>23.78409461006696</v>
+        <v>-23.78409461006696</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
@@ -650,10 +650,10 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-22.24107886174358</v>
+        <v>22.24107886174357</v>
       </c>
       <c r="B20" t="n">
-        <v>55.74834558300437</v>
+        <v>-55.74834558300439</v>
       </c>
       <c r="C20" t="n">
         <v>1</v>
@@ -661,10 +661,10 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>-33.97510633590858</v>
+        <v>33.97510633590857</v>
       </c>
       <c r="B21" t="n">
-        <v>-30.72203703806299</v>
+        <v>30.722037038063</v>
       </c>
       <c r="C21" t="n">
         <v>1</v>
@@ -672,10 +672,10 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>-43.90576614420566</v>
+        <v>43.90576614420564</v>
       </c>
       <c r="B22" t="n">
-        <v>23.11459317339699</v>
+        <v>-23.114593173397</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
@@ -683,10 +683,10 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>-22.6401763833145</v>
+        <v>22.6401763833145</v>
       </c>
       <c r="B23" t="n">
-        <v>56.00895921534405</v>
+        <v>-56.00895921534407</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>-33.72236509655497</v>
+        <v>33.72236509655497</v>
       </c>
       <c r="B24" t="n">
-        <v>-30.6826829690558</v>
+        <v>30.68268296905581</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
@@ -705,10 +705,10 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>-42.88575725458053</v>
+        <v>42.88575725458053</v>
       </c>
       <c r="B25" t="n">
-        <v>24.50814269726196</v>
+        <v>-24.50814269726197</v>
       </c>
       <c r="C25" t="n">
         <v>1</v>
@@ -716,10 +716,10 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>-22.83990860370458</v>
+        <v>22.83990860370458</v>
       </c>
       <c r="B26" t="n">
-        <v>56.48934482421512</v>
+        <v>-56.48934482421513</v>
       </c>
       <c r="C26" t="n">
         <v>1</v>
@@ -727,10 +727,10 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-46.64464959041609</v>
+        <v>46.64464959041608</v>
       </c>
       <c r="B27" t="n">
-        <v>77.27232414422168</v>
+        <v>-77.27232414422173</v>
       </c>
       <c r="C27" t="n">
         <v>2</v>
@@ -738,10 +738,10 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>-204.6111235130483</v>
+        <v>204.6111235130482</v>
       </c>
       <c r="B28" t="n">
-        <v>34.34135917735851</v>
+        <v>-34.34135917735852</v>
       </c>
       <c r="C28" t="n">
         <v>2</v>
@@ -749,10 +749,10 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-242.7918640018311</v>
+        <v>242.791864001831</v>
       </c>
       <c r="B29" t="n">
-        <v>5.399583334040809</v>
+        <v>-5.399583334040813</v>
       </c>
       <c r="C29" t="n">
         <v>2</v>
@@ -760,10 +760,10 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>-207.5071627221975</v>
+        <v>207.5071627221974</v>
       </c>
       <c r="B30" t="n">
-        <v>-53.79373917523522</v>
+        <v>53.79373917523524</v>
       </c>
       <c r="C30" t="n">
         <v>2</v>
@@ -771,10 +771,10 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>-191.0452012094882</v>
+        <v>191.0452012094882</v>
       </c>
       <c r="B31" t="n">
-        <v>-67.26311253095008</v>
+        <v>67.2631125309501</v>
       </c>
       <c r="C31" t="n">
         <v>2</v>
@@ -782,10 +782,10 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>-181.2236385963581</v>
+        <v>181.2236385963581</v>
       </c>
       <c r="B32" t="n">
-        <v>-69.91719393286873</v>
+        <v>69.91719393286874</v>
       </c>
       <c r="C32" t="n">
         <v>2</v>
@@ -793,10 +793,10 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>-184.7347997810601</v>
+        <v>184.73479978106</v>
       </c>
       <c r="B33" t="n">
-        <v>-72.57512592501675</v>
+        <v>72.57512592501678</v>
       </c>
       <c r="C33" t="n">
         <v>2</v>
@@ -804,10 +804,10 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>-94.76692141648326</v>
+        <v>94.76692141648324</v>
       </c>
       <c r="B34" t="n">
-        <v>-59.94085410569713</v>
+        <v>59.94085410569714</v>
       </c>
       <c r="C34" t="n">
         <v>2</v>
@@ -815,10 +815,10 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>-80.76858059347964</v>
+        <v>80.76858059347963</v>
       </c>
       <c r="B35" t="n">
-        <v>-45.48417748526481</v>
+        <v>45.48417748526482</v>
       </c>
       <c r="C35" t="n">
         <v>2</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>-78.02263138591996</v>
+        <v>78.02263138591995</v>
       </c>
       <c r="B36" t="n">
-        <v>-66.98925742493341</v>
+        <v>66.98925742493343</v>
       </c>
       <c r="C36" t="n">
         <v>2</v>
@@ -837,10 +837,10 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>-241.9944098317442</v>
+        <v>241.9944098317442</v>
       </c>
       <c r="B37" t="n">
-        <v>5.710334351748131</v>
+        <v>-5.710334351748137</v>
       </c>
       <c r="C37" t="n">
         <v>2</v>
@@ -848,10 +848,10 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>-205.5465410488142</v>
+        <v>205.5465410488141</v>
       </c>
       <c r="B38" t="n">
-        <v>34.40770169725734</v>
+        <v>-34.40770169725737</v>
       </c>
       <c r="C38" t="n">
         <v>2</v>
@@ -859,10 +859,10 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>-45.37154394486112</v>
+        <v>45.37154394486111</v>
       </c>
       <c r="B39" t="n">
-        <v>77.71824954124435</v>
+        <v>-77.71824954124436</v>
       </c>
       <c r="C39" t="n">
         <v>2</v>
@@ -870,10 +870,10 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>-244.600656698791</v>
+        <v>244.600656698791</v>
       </c>
       <c r="B40" t="n">
-        <v>5.343773879081223</v>
+        <v>-5.343773879081229</v>
       </c>
       <c r="C40" t="n">
         <v>2</v>
@@ -881,10 +881,10 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>-202.4549850797039</v>
+        <v>202.4549850797038</v>
       </c>
       <c r="B41" t="n">
-        <v>34.52179637043668</v>
+        <v>-34.52179637043669</v>
       </c>
       <c r="C41" t="n">
         <v>2</v>
@@ -892,10 +892,10 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>-46.2445756229962</v>
+        <v>46.24457562299619</v>
       </c>
       <c r="B42" t="n">
-        <v>77.73429930462639</v>
+        <v>-77.73429930462642</v>
       </c>
       <c r="C42" t="n">
         <v>2</v>
@@ -903,10 +903,10 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>-243.2544212442867</v>
+        <v>243.2544212442867</v>
       </c>
       <c r="B43" t="n">
-        <v>5.038837443312659</v>
+        <v>-5.038837443312665</v>
       </c>
       <c r="C43" t="n">
         <v>2</v>
@@ -914,10 +914,10 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>-202.8919953077075</v>
+        <v>202.8919953077074</v>
       </c>
       <c r="B44" t="n">
-        <v>34.43360737771535</v>
+        <v>-34.43360737771537</v>
       </c>
       <c r="C44" t="n">
         <v>2</v>
@@ -925,10 +925,10 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>-48.25576137824802</v>
+        <v>48.25576137824801</v>
       </c>
       <c r="B45" t="n">
-        <v>77.02144300597658</v>
+        <v>-77.02144300597661</v>
       </c>
       <c r="C45" t="n">
         <v>2</v>
@@ -936,10 +936,10 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>-243.6678471207607</v>
+        <v>243.6678471207606</v>
       </c>
       <c r="B46" t="n">
-        <v>5.497095720359944</v>
+        <v>-5.497095720359951</v>
       </c>
       <c r="C46" t="n">
         <v>2</v>
@@ -947,10 +947,10 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>-203.7444567600447</v>
+        <v>203.7444567600446</v>
       </c>
       <c r="B47" t="n">
-        <v>34.47718257981344</v>
+        <v>-34.47718257981345</v>
       </c>
       <c r="C47" t="n">
         <v>2</v>
@@ -958,10 +958,10 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>-47.68925121723033</v>
+        <v>47.68925121723031</v>
       </c>
       <c r="B48" t="n">
-        <v>77.0279642951444</v>
+        <v>-77.02796429514441</v>
       </c>
       <c r="C48" t="n">
         <v>2</v>
@@ -969,10 +969,10 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>-244.753444092229</v>
+        <v>244.753444092229</v>
       </c>
       <c r="B49" t="n">
-        <v>4.818607313485096</v>
+        <v>-4.8186073134851</v>
       </c>
       <c r="C49" t="n">
         <v>2</v>
@@ -980,10 +980,10 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>-201.7702559551056</v>
+        <v>201.7702559551056</v>
       </c>
       <c r="B50" t="n">
-        <v>34.99790505699496</v>
+        <v>-34.99790505699498</v>
       </c>
       <c r="C50" t="n">
         <v>2</v>
@@ -991,10 +991,10 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>-47.56465293619552</v>
+        <v>47.56465293619551</v>
       </c>
       <c r="B51" t="n">
-        <v>76.96093547347532</v>
+        <v>-76.96093547347535</v>
       </c>
       <c r="C51" t="n">
         <v>2</v>
@@ -1002,10 +1002,10 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>151.0940430931604</v>
+        <v>-151.0940430931603</v>
       </c>
       <c r="B52" t="n">
-        <v>59.95028446452335</v>
+        <v>-59.95028446452336</v>
       </c>
       <c r="C52" t="n">
         <v>3</v>
@@ -1013,10 +1013,10 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>183.4403339199195</v>
+        <v>-183.4403339199195</v>
       </c>
       <c r="B53" t="n">
-        <v>31.6416146917306</v>
+        <v>-31.6416146917306</v>
       </c>
       <c r="C53" t="n">
         <v>3</v>
@@ -1024,10 +1024,10 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>212.7012446593912</v>
+        <v>-212.7012446593911</v>
       </c>
       <c r="B54" t="n">
-        <v>-5.135791612638149</v>
+        <v>5.135791612638164</v>
       </c>
       <c r="C54" t="n">
         <v>3</v>
@@ -1035,10 +1035,10 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>234.8783794805105</v>
+        <v>-234.8783794805104</v>
       </c>
       <c r="B55" t="n">
-        <v>-5.533155899488206</v>
+        <v>5.533155899488222</v>
       </c>
       <c r="C55" t="n">
         <v>3</v>
@@ -1046,10 +1046,10 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>237.2371440164432</v>
+        <v>-237.2371440164432</v>
       </c>
       <c r="B56" t="n">
-        <v>-56.67243603083974</v>
+        <v>56.67243603083977</v>
       </c>
       <c r="C56" t="n">
         <v>3</v>
@@ -1057,10 +1057,10 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>237.5868694833789</v>
+        <v>-237.5868694833788</v>
       </c>
       <c r="B57" t="n">
-        <v>-74.56048887874402</v>
+        <v>74.56048887874405</v>
       </c>
       <c r="C57" t="n">
         <v>3</v>
@@ -1068,10 +1068,10 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>238.2110762227871</v>
+        <v>-238.211076222787</v>
       </c>
       <c r="B58" t="n">
-        <v>-73.52693939817118</v>
+        <v>73.52693939817121</v>
       </c>
       <c r="C58" t="n">
         <v>3</v>
@@ -1079,10 +1079,10 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>238.5072291916437</v>
+        <v>-238.5072291916436</v>
       </c>
       <c r="B59" t="n">
-        <v>-73.65970298305442</v>
+        <v>73.65970298305446</v>
       </c>
       <c r="C59" t="n">
         <v>3</v>
@@ -1090,10 +1090,10 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>240.2080190716331</v>
+        <v>-240.208019071633</v>
       </c>
       <c r="B60" t="n">
-        <v>-75.14042885451151</v>
+        <v>75.14042885451154</v>
       </c>
       <c r="C60" t="n">
         <v>3</v>
@@ -1101,10 +1101,10 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>240.5605929758893</v>
+        <v>-240.5605929758892</v>
       </c>
       <c r="B61" t="n">
-        <v>-84.89379608371981</v>
+        <v>84.89379608371982</v>
       </c>
       <c r="C61" t="n">
         <v>3</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>213.0764002147653</v>
+        <v>-213.0764002147652</v>
       </c>
       <c r="B62" t="n">
-        <v>-5.147134617352016</v>
+        <v>5.147134617352033</v>
       </c>
       <c r="C62" t="n">
         <v>3</v>
@@ -1123,10 +1123,10 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>183.6352825227975</v>
+        <v>-183.6352825227974</v>
       </c>
       <c r="B63" t="n">
-        <v>31.6686150162398</v>
+        <v>-31.6686150162398</v>
       </c>
       <c r="C63" t="n">
         <v>3</v>
@@ -1134,10 +1134,10 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>151.3514581631626</v>
+        <v>-151.3514581631625</v>
       </c>
       <c r="B64" t="n">
-        <v>60.6866176188073</v>
+        <v>-60.68661761880731</v>
       </c>
       <c r="C64" t="n">
         <v>3</v>
@@ -1145,10 +1145,10 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>212.5119001053075</v>
+        <v>-212.5119001053074</v>
       </c>
       <c r="B65" t="n">
-        <v>-4.94567733319324</v>
+        <v>4.94567733319325</v>
       </c>
       <c r="C65" t="n">
         <v>3</v>
@@ -1156,10 +1156,10 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>184.2558729954787</v>
+        <v>-184.2558729954786</v>
       </c>
       <c r="B66" t="n">
-        <v>33.00452757324562</v>
+        <v>-33.00452757324563</v>
       </c>
       <c r="C66" t="n">
         <v>3</v>
@@ -1167,10 +1167,10 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>152.0504885054204</v>
+        <v>-152.0504885054203</v>
       </c>
       <c r="B67" t="n">
-        <v>59.21444910971277</v>
+        <v>-59.21444910971279</v>
       </c>
       <c r="C67" t="n">
         <v>3</v>
@@ -1178,10 +1178,10 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>213.2754310431901</v>
+        <v>-213.27543104319</v>
       </c>
       <c r="B68" t="n">
-        <v>-4.800725859616033</v>
+        <v>4.800725859616044</v>
       </c>
       <c r="C68" t="n">
         <v>3</v>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>184.1648396893999</v>
+        <v>-184.1648396893998</v>
       </c>
       <c r="B69" t="n">
-        <v>32.1019478737936</v>
+        <v>-32.1019478737936</v>
       </c>
       <c r="C69" t="n">
         <v>3</v>
@@ -1200,10 +1200,10 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>150.6914893976013</v>
+        <v>-150.6914893976012</v>
       </c>
       <c r="B70" t="n">
-        <v>59.06342363955447</v>
+        <v>-59.06342363955449</v>
       </c>
       <c r="C70" t="n">
         <v>3</v>
@@ -1211,10 +1211,10 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>213.0921113672619</v>
+        <v>-213.0921113672618</v>
       </c>
       <c r="B71" t="n">
-        <v>-5.310156941893606</v>
+        <v>5.310156941893615</v>
       </c>
       <c r="C71" t="n">
         <v>3</v>
@@ -1222,10 +1222,10 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>183.8322746961004</v>
+        <v>-183.8322746961003</v>
       </c>
       <c r="B72" t="n">
-        <v>31.29371860763054</v>
+        <v>-31.29371860763054</v>
       </c>
       <c r="C72" t="n">
         <v>3</v>
@@ -1233,10 +1233,10 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>150.9773576786609</v>
+        <v>-150.9773576786609</v>
       </c>
       <c r="B73" t="n">
-        <v>59.69075689436247</v>
+        <v>-59.69075689436248</v>
       </c>
       <c r="C73" t="n">
         <v>3</v>
@@ -1244,10 +1244,10 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>212.8367125781968</v>
+        <v>-212.8367125781967</v>
       </c>
       <c r="B74" t="n">
-        <v>-5.167266813379257</v>
+        <v>5.167266813379273</v>
       </c>
       <c r="C74" t="n">
         <v>3</v>
@@ -1255,10 +1255,10 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>184.0348571069301</v>
+        <v>-184.0348571069301</v>
       </c>
       <c r="B75" t="n">
-        <v>32.1024715515917</v>
+        <v>-32.10247155159171</v>
       </c>
       <c r="C75" t="n">
         <v>3</v>
@@ -1266,10 +1266,10 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>151.1522359317105</v>
+        <v>-151.1522359317104</v>
       </c>
       <c r="B76" t="n">
-        <v>60.19886657309839</v>
+        <v>-60.1988665730984</v>
       </c>
       <c r="C76" t="n">
         <v>3</v>

</xml_diff>